<commit_message>
feat: Modified functional test case for create profiles and added time taken for processing files
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/CaseWorkerUserWithNoPassword.xlsx
+++ b/src/functionalTest/resources/CaseWorkerUserWithNoPassword.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B8564A-4BDD-F64C-A907-04B813050422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A134DEFE-693E-EA49-9F9E-EB2E53B68BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caseworker Roles" sheetId="11" state="hidden" r:id="rId1"/>
@@ -22,10 +22,19 @@
     <sheet name="Roles" sheetId="4" r:id="rId7"/>
     <sheet name="Validations" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -156,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="1266">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -4054,13 +4063,16 @@
     <t>AAI</t>
   </si>
   <si>
-    <t>test1@hmcts.net</t>
-  </si>
-  <si>
-    <t>test2@hmcts.net</t>
-  </si>
-  <si>
-    <t>test3@hmcts.net</t>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Waugh</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Smith</t>
   </si>
 </sst>
 </file>
@@ -8978,13 +8990,13 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="62.5" customWidth="1"/>
     <col min="7" max="7" width="33.83203125" hidden="1" customWidth="1"/>
@@ -9110,8 +9122,9 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1262</v>
+      <c r="C2" s="3" t="str">
+        <f ca="1">CONCATENATE(A2,".",B2,"@","crdfunctestuser",RANDBETWEEN(1,999),".com")</f>
+        <v>Joe.Bloggs@crdfunctestuser89.com</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
@@ -9197,13 +9210,14 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>1262</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>1263</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C4" ca="1" si="0">CONCATENATE(A3,".",B3,"@","crdfunctestuser",RANDBETWEEN(1,999),".com")</f>
+        <v>Mark.Waugh@crdfunctestuser487.com</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -9265,33 +9279,34 @@
         <v>1253</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>1253</v>
+        <v>1257</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>1253</v>
+        <v>1258</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>1253</v>
+        <v>1260</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>1253</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>1264</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1264</v>
+        <v>1265</v>
+      </c>
+      <c r="C4" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Steve.Smith@crdfunctestuser780.com</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -9353,34 +9368,32 @@
         <v>1253</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>1253</v>
+        <v>1257</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>1253</v>
+        <v>1258</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>1253</v>
+        <v>1260</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>1253</v>
+        <v>1261</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C3:C4" r:id="rId2" display="test@hmcts.net" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{471034CF-581E-3840-8E11-F18387A628CE}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{8E38AD4B-FA70-3D4C-8BC3-B46C72088724}"/>
+    <hyperlink ref="C2" r:id="rId1" display="test1@hmcts.net" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3:C4" r:id="rId2" display="test1@hmcts.net" xr:uid="{6D510A2A-83A0-6F46-8D21-5F4FC391B357}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">

</xml_diff>